<commit_message>
Small update to the dwemer table
</commit_message>
<xml_diff>
--- a/Files/Modules/Dwemer Legacy/Tables/Equipment/Armor.xlsx
+++ b/Files/Modules/Dwemer Legacy/Tables/Equipment/Armor.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091B87C9-1AE7-4215-A3EB-BC3BA35EE753}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="60">
   <si>
     <t>ARMOR</t>
   </si>
@@ -184,12 +185,27 @@
   </si>
   <si>
     <t>Exotic</t>
+  </si>
+  <si>
+    <t>Dwemer Kragen Helm</t>
+  </si>
+  <si>
+    <t>Dwemer Kragen Cuirass</t>
+  </si>
+  <si>
+    <t>Dwemer Kragen Gauntlets</t>
+  </si>
+  <si>
+    <t>Dwemer Kragen Boots</t>
+  </si>
+  <si>
+    <t>Dwemer Kragen Shield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,8 +244,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{1D2B4921-04FD-443A-956E-BA0C54D9A434}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -503,11 +547,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,6 +1050,61 @@
         <v>54</v>
       </c>
     </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:I3"/>

</xml_diff>

<commit_message>
Dwemer module small update
</commit_message>
<xml_diff>
--- a/Files/Modules/Dwemer Legacy/Tables/Equipment/Armor.xlsx
+++ b/Files/Modules/Dwemer Legacy/Tables/Equipment/Armor.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B7F5E835-A312-44C1-BD61-6EA93BF41EBC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C051DAE8-35D7-4C14-A0B3-EB6D90DAB371}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="100">
   <si>
     <t>ARMOR</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>Dwemer Scout Outfit</t>
+  </si>
+  <si>
+    <t>Dwemer Juggernaut Helm</t>
+  </si>
+  <si>
+    <t>Dwemer Juggernaut Cuirass</t>
+  </si>
+  <si>
+    <t>Dwemer Juggernaut Gauntlets</t>
+  </si>
+  <si>
+    <t>Dwemer Juggernaut Boots</t>
   </si>
 </sst>
 </file>
@@ -656,10 +668,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I81"/>
+  <dimension ref="B2:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,6 +1547,50 @@
         <v>54</v>
       </c>
     </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C82" t="s">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>12</v>
+      </c>
+      <c r="D83" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:I3"/>

</xml_diff>